<commit_message>
Charge 17 - Updated Mg inventory
</commit_message>
<xml_diff>
--- a/Charge 17 - C07.xlsx
+++ b/Charge 17 - C07.xlsx
@@ -8580,7 +8580,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="166">
-        <v>5.6260000000000003</v>
+        <v>5.4009999999999998</v>
       </c>
       <c r="B3" s="125">
         <v>0</v>
@@ -8600,7 +8600,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="166">
-        <v>5.64</v>
+        <v>5.5540000000000003</v>
       </c>
       <c r="B4" s="125">
         <v>0</v>
@@ -8620,7 +8620,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="166">
-        <v>5.9320000000000004</v>
+        <v>5.6260000000000003</v>
       </c>
       <c r="B5" s="125">
         <v>0</v>
@@ -8632,7 +8632,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="166">
-        <v>6.5289999999999999</v>
+        <v>5.64</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
@@ -8645,7 +8645,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="166">
-        <v>6.7119999999999997</v>
+        <v>5.7</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
@@ -8657,7 +8657,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="166">
-        <v>7.7039999999999997</v>
+        <v>5.9320000000000004</v>
       </c>
       <c r="B8" s="125">
         <v>0</v>
@@ -8670,7 +8670,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="166">
-        <v>8.8819999999999997</v>
+        <v>6.2210000000000001</v>
       </c>
       <c r="B9" s="125">
         <v>0</v>
@@ -8681,7 +8681,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="166"/>
+      <c r="A10" s="166">
+        <v>6.4550000000000001</v>
+      </c>
       <c r="B10" s="125">
         <v>0</v>
       </c>
@@ -8691,7 +8693,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="166"/>
+      <c r="A11" s="166">
+        <v>6.5289999999999999</v>
+      </c>
       <c r="B11" s="125">
         <v>0</v>
       </c>
@@ -8701,7 +8705,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="166"/>
+      <c r="A12" s="166">
+        <v>6.7119999999999997</v>
+      </c>
       <c r="B12" s="125">
         <v>0</v>
       </c>
@@ -8711,7 +8717,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="166"/>
+      <c r="A13" s="166">
+        <v>6.8869999999999996</v>
+      </c>
       <c r="B13" s="125">
         <v>0</v>
       </c>
@@ -8721,7 +8729,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="166"/>
+      <c r="A14" s="166">
+        <v>7.1079999999999997</v>
+      </c>
       <c r="B14" s="125">
         <v>0</v>
       </c>
@@ -8731,7 +8741,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="166"/>
+      <c r="A15" s="166">
+        <v>7.2359999999999998</v>
+      </c>
       <c r="B15" s="125">
         <v>0</v>
       </c>
@@ -8741,7 +8753,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="166"/>
+      <c r="A16" s="166">
+        <v>7.26</v>
+      </c>
       <c r="B16" s="125">
         <v>0</v>
       </c>
@@ -8751,7 +8765,9 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="166"/>
+      <c r="A17" s="166">
+        <v>7.3710000000000004</v>
+      </c>
       <c r="B17" s="125">
         <v>0</v>
       </c>
@@ -8761,7 +8777,9 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="166"/>
+      <c r="A18" s="166">
+        <v>7.4859999999999998</v>
+      </c>
       <c r="B18" s="125">
         <v>0</v>
       </c>
@@ -8771,7 +8789,9 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="166"/>
+      <c r="A19" s="166">
+        <v>7.7039999999999997</v>
+      </c>
       <c r="B19" s="125">
         <v>0</v>
       </c>
@@ -8781,7 +8801,9 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="166"/>
+      <c r="A20" s="166">
+        <v>7.7169999999999996</v>
+      </c>
       <c r="B20" s="125">
         <v>0</v>
       </c>
@@ -8791,7 +8813,9 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="166"/>
+      <c r="A21" s="166">
+        <v>7.75</v>
+      </c>
       <c r="B21" s="125">
         <v>0</v>
       </c>
@@ -8801,7 +8825,9 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="166"/>
+      <c r="A22" s="166">
+        <v>8.8819999999999997</v>
+      </c>
       <c r="B22" s="125">
         <v>0</v>
       </c>
@@ -8811,7 +8837,9 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="166"/>
+      <c r="A23" s="166">
+        <v>8.8970000000000002</v>
+      </c>
       <c r="B23" s="125">
         <v>0</v>
       </c>
@@ -8821,7 +8849,9 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="166"/>
+      <c r="A24" s="166">
+        <v>11.073</v>
+      </c>
       <c r="B24" s="125">
         <v>0</v>
       </c>
@@ -8831,7 +8861,9 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="166"/>
+      <c r="A25" s="166">
+        <v>11.09</v>
+      </c>
       <c r="B25" s="125">
         <v>0</v>
       </c>
@@ -8841,7 +8873,9 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="166"/>
+      <c r="A26" s="166">
+        <v>11.398</v>
+      </c>
       <c r="B26" s="125">
         <v>0</v>
       </c>
@@ -8851,7 +8885,9 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="166"/>
+      <c r="A27" s="166">
+        <v>12.666</v>
+      </c>
       <c r="B27" s="125">
         <v>0</v>
       </c>
@@ -9161,7 +9197,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
         <v>0</v>
       </c>
       <c r="D2">
@@ -9184,7 +9220,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E3" s="50" t="s">
@@ -9203,7 +9239,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="50" t="s">
@@ -9222,7 +9258,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9234,7 +9270,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9246,7 +9282,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9258,7 +9294,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9270,7 +9306,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9282,7 +9318,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9294,7 +9330,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9306,7 +9342,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9318,7 +9354,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9330,7 +9366,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9342,7 +9378,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9354,7 +9390,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9366,7 +9402,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9378,7 +9414,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9388,7 +9424,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9398,7 +9434,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9408,7 +9444,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9418,7 +9454,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9428,7 +9464,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9438,7 +9474,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9448,7 +9484,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9458,7 +9494,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9468,7 +9504,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9478,7 +9514,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9488,7 +9524,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9498,7 +9534,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9508,7 +9544,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9518,7 +9554,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9528,7 +9564,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9538,7 +9574,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C65" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -9548,7 +9584,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9558,7 +9594,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9568,7 +9604,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9578,7 +9614,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9588,7 +9624,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9598,7 +9634,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9608,7 +9644,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9618,7 +9654,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9628,7 +9664,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9638,7 +9674,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9648,7 +9684,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9658,7 +9694,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9668,7 +9704,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9678,7 +9714,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9688,7 +9724,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9698,7 +9734,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9708,7 +9744,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cast Charge 17 and created Charge 18
</commit_message>
<xml_diff>
--- a/Charge 17 - C07.xlsx
+++ b/Charge 17 - C07.xlsx
@@ -4918,9 +4918,9 @@
       <c r="G2" s="175"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="173" t="e">
+      <c r="A3" s="173" t="str">
         <f>"Actual  " &amp; 'Charge 17'!I3</f>
-        <v>#DIV/0!</v>
+        <v>Actual  Mg65Zn30Ca5</v>
       </c>
       <c r="B3" s="174"/>
       <c r="C3" s="174"/>
@@ -4982,17 +4982,17 @@
       <c r="A6" s="26">
         <v>1</v>
       </c>
-      <c r="B6" s="105" t="str">
+      <c r="B6" s="105">
         <f>IF('Charge 17'!B14=0, "-", 'Charge 17'!B14)</f>
-        <v>-</v>
-      </c>
-      <c r="C6" s="137" t="str">
+        <v>7.7039999999999997</v>
+      </c>
+      <c r="C6" s="137">
         <f>IF('Charge 17'!E14=0,"-",'Charge 17'!E14)</f>
-        <v>-</v>
-      </c>
-      <c r="D6" s="137" t="str">
+        <v>17.132999999999999</v>
+      </c>
+      <c r="D6" s="137">
         <f>IF('Charge 17'!H14=0, "-", 'Charge 17'!H14)</f>
-        <v>-</v>
+        <v>3.5110000000000001</v>
       </c>
       <c r="E6" s="137" t="str">
         <f>IF('Charge 17'!K14=0, "-", 'Charge 17'!K14)</f>
@@ -5004,7 +5004,7 @@
       </c>
       <c r="G6" s="138">
         <f>COUNTIF(B6:B20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="131" t="str">
         <f>B4</f>
@@ -5015,13 +5015,13 @@
       <c r="A7" s="27">
         <v>2</v>
       </c>
-      <c r="B7" s="108" t="str">
+      <c r="B7" s="108">
         <f>IF('Charge 17'!B15=0, "-", 'Charge 17'!B15)</f>
-        <v>-</v>
-      </c>
-      <c r="C7" s="107" t="str">
+        <v>8.8970000000000002</v>
+      </c>
+      <c r="C7" s="107">
         <f>IF('Charge 17'!E15=0,"-",'Charge 17'!E15)</f>
-        <v>-</v>
+        <v>17.224</v>
       </c>
       <c r="D7" s="107" t="str">
         <f>IF('Charge 17'!H15=0, "-", 'Charge 17'!H15)</f>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="G7" s="106">
         <f>COUNTIF(C6:C20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="151" t="str">
         <f>C4</f>
@@ -5048,9 +5048,9 @@
       <c r="A8" s="27">
         <v>3</v>
       </c>
-      <c r="B8" s="108" t="str">
+      <c r="B8" s="108">
         <f>IF('Charge 17'!B16=0, "-", 'Charge 17'!B16)</f>
-        <v>-</v>
+        <v>11.073</v>
       </c>
       <c r="C8" s="107" t="str">
         <f>IF('Charge 17'!E16=0,"-",'Charge 17'!E16)</f>
@@ -5070,7 +5070,7 @@
       </c>
       <c r="G8" s="106">
         <f>COUNTIF(D6:D20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="148" t="str">
         <f>D4</f>
@@ -5169,7 +5169,7 @@
       </c>
       <c r="G11" s="160">
         <f>COUNTIF(B6:F20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H11" s="153" t="str">
         <f>G4</f>
@@ -5416,15 +5416,15 @@
       </c>
       <c r="B21" s="77">
         <f>SUM(B6:B20)</f>
-        <v>0</v>
+        <v>27.673999999999999</v>
       </c>
       <c r="C21" s="37">
         <f>SUM(C6:C20)</f>
-        <v>0</v>
+        <v>34.356999999999999</v>
       </c>
       <c r="D21" s="69">
         <f>SUM(D6:D20)</f>
-        <v>0</v>
+        <v>3.5110000000000001</v>
       </c>
       <c r="E21" s="69">
         <f>SUM(E6:E20)</f>
@@ -5436,7 +5436,7 @@
       </c>
       <c r="G21" s="144">
         <f>SUM(B21:F21)</f>
-        <v>0</v>
+        <v>65.542000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5445,15 +5445,15 @@
       </c>
       <c r="B22" s="145">
         <f>'Charge 17'!F4</f>
-        <v>54.823999999999998</v>
+        <v>27.677</v>
       </c>
       <c r="C22" s="135">
         <f>'Charge 17'!F5</f>
-        <v>68.067999999999998</v>
+        <v>34.363</v>
       </c>
       <c r="D22" s="135">
         <f>'Charge 17'!F6</f>
-        <v>6.9539999999999997</v>
+        <v>3.5110000000000001</v>
       </c>
       <c r="E22" s="135">
         <f>'Charge 17'!F7</f>
@@ -5465,7 +5465,7 @@
       </c>
       <c r="G22" s="70">
         <f>SUM(B22:F22)</f>
-        <v>129.846</v>
+        <v>65.551000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5474,15 +5474,15 @@
       </c>
       <c r="B23" s="146">
         <f>B21-B22</f>
-        <v>-54.823999999999998</v>
+        <v>-3.0000000000001137E-3</v>
       </c>
       <c r="C23" s="140">
         <f t="shared" ref="C23:G23" si="0">C21-C22</f>
-        <v>-68.067999999999998</v>
+        <v>-6.0000000000002274E-3</v>
       </c>
       <c r="D23" s="140">
         <f t="shared" si="0"/>
-        <v>-6.9539999999999997</v>
+        <v>0</v>
       </c>
       <c r="E23" s="140">
         <f t="shared" si="0"/>
@@ -5494,7 +5494,7 @@
       </c>
       <c r="G23" s="113">
         <f t="shared" si="0"/>
-        <v>-129.846</v>
+        <v>-9.0000000000003411E-3</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -5588,9 +5588,9 @@
       <c r="G3" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="62" t="e">
+      <c r="I3" s="62" t="str">
         <f>Q4 &amp; ROUND(N4,3)*100 &amp; IF(N5=0, "", Q5 &amp; ROUND(N5,3)*100) &amp; IF(N6=0, "", Q6 &amp; ROUND(N6,3)*100) &amp; IF(N7=0, "", Q7 &amp; ROUND(N7,3)*100) &amp; IF(N8=0, "", Q8 &amp; ROUND(N8,3)*100)</f>
-        <v>#DIV/0!</v>
+        <v>Mg65Zn30Ca5</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="s">
@@ -5683,11 +5683,11 @@
       </c>
       <c r="F4" s="69">
         <f>IF($F$9=0, ROUND($F$10*E4, 3), ROUND(E4*$F$9, 3))</f>
-        <v>54.823999999999998</v>
+        <v>27.677</v>
       </c>
       <c r="G4" s="70">
         <f>IFERROR(F4/U4, 0)</f>
-        <v>31.544303797468352</v>
+        <v>15.924626006904488</v>
       </c>
       <c r="I4" s="71" t="str">
         <f>$Q$4</f>
@@ -5696,19 +5696,19 @@
       <c r="J4" s="26"/>
       <c r="K4" s="72">
         <f>B29</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="73" t="e">
+        <v>27.673999999999999</v>
+      </c>
+      <c r="L4" s="73">
         <f>K4/$K$9</f>
-        <v>#DIV/0!</v>
+        <v>0.42223307192334686</v>
       </c>
       <c r="M4" s="23">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="115" t="e">
+        <v>1.7372272039635747E-2</v>
+      </c>
+      <c r="N4" s="115">
         <f>M4/$M$9</f>
-        <v>#DIV/0!</v>
+        <v>0.65000532893542873</v>
       </c>
       <c r="P4" s="15">
         <v>1</v>
@@ -5780,11 +5780,11 @@
       </c>
       <c r="F5" s="69">
         <f t="shared" ref="F5:F8" si="0">IF($F$9=0, ROUND($F$10*E5, 3), ROUND(E5*$F$9, 3))</f>
-        <v>68.067999999999998</v>
+        <v>34.363</v>
       </c>
       <c r="G5" s="70">
         <f>IFERROR(F5/U5, 0)</f>
-        <v>9.5333333333333332</v>
+        <v>4.8127450980392155</v>
       </c>
       <c r="I5" s="71" t="str">
         <f>$Q$5</f>
@@ -5793,19 +5793,19 @@
       <c r="J5" s="27"/>
       <c r="K5" s="75">
         <f>E29</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="76" t="e">
+        <v>34.356999999999999</v>
+      </c>
+      <c r="L5" s="76">
         <f>K5/$K$9</f>
-        <v>#DIV/0!</v>
+        <v>0.52419822403954719</v>
       </c>
       <c r="M5" s="24">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="116" t="e">
+        <v>8.0174700076404391E-3</v>
+      </c>
+      <c r="N5" s="116">
         <f>M5/$M$9</f>
-        <v>#DIV/0!</v>
+        <v>0.29998368766366201</v>
       </c>
       <c r="P5" s="15">
         <v>2</v>
@@ -5877,11 +5877,11 @@
       </c>
       <c r="F6" s="69">
         <f t="shared" si="0"/>
-        <v>6.9539999999999997</v>
+        <v>3.5110000000000001</v>
       </c>
       <c r="G6" s="70">
         <f>IFERROR(F6/U6, 0)</f>
-        <v>4.4864516129032257</v>
+        <v>2.2651612903225806</v>
       </c>
       <c r="I6" s="71" t="str">
         <f>$Q$6</f>
@@ -5890,19 +5890,19 @@
       <c r="J6" s="27"/>
       <c r="K6" s="77">
         <f>H29</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="76" t="e">
+        <v>3.5110000000000001</v>
+      </c>
+      <c r="L6" s="76">
         <f>K6/$K$9</f>
-        <v>#DIV/0!</v>
+        <v>5.356870403710598E-2</v>
       </c>
       <c r="M6" s="24">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="116" t="e">
+        <v>1.3366112090699629E-3</v>
+      </c>
+      <c r="N6" s="116">
         <f>M6/$M$9</f>
-        <v>#DIV/0!</v>
+        <v>5.0010983400909197E-2</v>
       </c>
       <c r="P6" s="15">
         <v>3</v>
@@ -5989,17 +5989,17 @@
         <f>K29</f>
         <v>0</v>
       </c>
-      <c r="L7" s="76" t="e">
+      <c r="L7" s="76">
         <f>K7/$K$9</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M7" s="24">
         <f>IFERROR(L7/T7, 0)</f>
         <v>0</v>
       </c>
-      <c r="N7" s="116" t="e">
+      <c r="N7" s="116">
         <f>M7/$M$9</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P7" s="15">
         <v>4</v>
@@ -6086,17 +6086,17 @@
         <f>N29</f>
         <v>0</v>
       </c>
-      <c r="L8" s="76" t="e">
+      <c r="L8" s="76">
         <f>K8/$K$9</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M8" s="24">
         <f>IFERROR(L8/T8, 0)</f>
         <v>0</v>
       </c>
-      <c r="N8" s="116" t="e">
+      <c r="N8" s="116">
         <f>M8/$M$9</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P8" s="18">
         <v>5</v>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="G9" s="144">
         <f>SUM(G4:G8)</f>
-        <v>45.564088743704907</v>
+        <v>23.002532395266286</v>
       </c>
       <c r="I9" s="82"/>
       <c r="J9" s="79" t="s">
@@ -6178,19 +6178,19 @@
       </c>
       <c r="K9" s="117">
         <f>SUM(K4:K8)</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="83" t="e">
+        <v>65.542000000000002</v>
+      </c>
+      <c r="L9" s="83">
         <f>SUM(L4:L8)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M9" s="118">
         <f>SUM(M4:M8)</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="84" t="e">
+        <v>2.672635325634615E-2</v>
+      </c>
+      <c r="N9" s="84">
         <f>SUM(N4:N8)</f>
-        <v>#DIV/0!</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>111</v>
@@ -6232,10 +6232,10 @@
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F10" s="158">
         <f>G10*U9</f>
-        <v>129.846</v>
+        <v>65.55</v>
       </c>
       <c r="G10" s="9">
-        <v>45.56</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="26.25" x14ac:dyDescent="0.4">
@@ -6341,7 +6341,7 @@
       </c>
       <c r="B14" s="106">
         <f>A!C2</f>
-        <v>0</v>
+        <v>7.7039999999999997</v>
       </c>
       <c r="C14" s="107"/>
       <c r="D14" s="126">
@@ -6349,7 +6349,7 @@
       </c>
       <c r="E14" s="106">
         <f>B!C2</f>
-        <v>0</v>
+        <v>17.132999999999999</v>
       </c>
       <c r="F14" s="107"/>
       <c r="G14" s="126">
@@ -6357,7 +6357,7 @@
       </c>
       <c r="H14" s="106">
         <f>'C'!C2</f>
-        <v>0</v>
+        <v>3.5110000000000001</v>
       </c>
       <c r="I14" s="107"/>
       <c r="J14" s="126">
@@ -6394,7 +6394,7 @@
       </c>
       <c r="B15" s="106">
         <f>A!C3</f>
-        <v>0</v>
+        <v>8.8970000000000002</v>
       </c>
       <c r="C15" s="107"/>
       <c r="D15" s="126">
@@ -6402,7 +6402,7 @@
       </c>
       <c r="E15" s="106">
         <f>B!C3</f>
-        <v>0</v>
+        <v>17.224</v>
       </c>
       <c r="F15" s="107"/>
       <c r="G15" s="126">
@@ -6447,7 +6447,7 @@
       </c>
       <c r="B16" s="106">
         <f>A!C4</f>
-        <v>0</v>
+        <v>11.073</v>
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="126">
@@ -7059,7 +7059,7 @@
       </c>
       <c r="B29" s="110">
         <f>SUM(B14:B28)</f>
-        <v>0</v>
+        <v>27.673999999999999</v>
       </c>
       <c r="C29" s="107"/>
       <c r="D29" s="109" t="s">
@@ -7067,7 +7067,7 @@
       </c>
       <c r="E29" s="111">
         <f>SUM(E14:E28)</f>
-        <v>0</v>
+        <v>34.356999999999999</v>
       </c>
       <c r="F29" s="107"/>
       <c r="G29" s="109" t="s">
@@ -7075,7 +7075,7 @@
       </c>
       <c r="H29" s="110">
         <f>SUM(H14:H28)</f>
-        <v>0</v>
+        <v>3.5110000000000001</v>
       </c>
       <c r="I29" s="107"/>
       <c r="J29" s="109" t="s">
@@ -7100,7 +7100,7 @@
       </c>
       <c r="B30" s="113">
         <f>B29-$F$4</f>
-        <v>-54.823999999999998</v>
+        <v>-3.0000000000001137E-3</v>
       </c>
       <c r="C30" s="114"/>
       <c r="D30" s="112" t="s">
@@ -7108,7 +7108,7 @@
       </c>
       <c r="E30" s="113">
         <f>E29-$F$5</f>
-        <v>-68.067999999999998</v>
+        <v>-6.0000000000002274E-3</v>
       </c>
       <c r="F30" s="114"/>
       <c r="G30" s="112" t="s">
@@ -7116,7 +7116,7 @@
       </c>
       <c r="H30" s="113">
         <f>H29-$F$6</f>
-        <v>-6.9539999999999997</v>
+        <v>0</v>
       </c>
       <c r="I30" s="114"/>
       <c r="J30" s="112" t="s">
@@ -8522,7 +8522,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -8557,37 +8557,37 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="166">
-        <v>3.9849999999999999</v>
+        <v>7.7039999999999997</v>
       </c>
       <c r="B2" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
+        <v>7.7039999999999997</v>
       </c>
       <c r="D2" s="1">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>27.673999999999999</v>
       </c>
       <c r="E2" s="127" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="129">
         <f>'Charge 17'!F4</f>
-        <v>54.823999999999998</v>
+        <v>27.677</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="166">
-        <v>5.4009999999999998</v>
+        <v>8.8970000000000002</v>
       </c>
       <c r="B3" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8.8970000000000002</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="127" t="s">
@@ -8595,19 +8595,19 @@
       </c>
       <c r="F3" s="129">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>27.673999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="166">
-        <v>5.5540000000000003</v>
+        <v>11.073</v>
       </c>
       <c r="B4" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>11.073</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="127" t="s">
@@ -8615,248 +8615,248 @@
       </c>
       <c r="F4" s="129">
         <f>F3-F2</f>
-        <v>-54.823999999999998</v>
+        <v>-3.0000000000001137E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="166">
-        <v>5.6260000000000003</v>
+        <v>3.9849999999999999</v>
       </c>
       <c r="B5" s="125">
         <v>0</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="166">
-        <v>5.64</v>
+        <v>5.4009999999999998</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="167"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="166">
-        <v>5.7</v>
+        <v>5.5540000000000003</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="166">
-        <v>5.9320000000000004</v>
+        <v>5.6260000000000003</v>
       </c>
       <c r="B8" s="125">
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8" s="167"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="166">
-        <v>6.2210000000000001</v>
+        <v>5.64</v>
       </c>
       <c r="B9" s="125">
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="166">
-        <v>6.4550000000000001</v>
+        <v>5.7</v>
       </c>
       <c r="B10" s="125">
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="166">
-        <v>6.5289999999999999</v>
+        <v>5.9320000000000004</v>
       </c>
       <c r="B11" s="125">
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="166">
-        <v>6.7119999999999997</v>
+        <v>6.2210000000000001</v>
       </c>
       <c r="B12" s="125">
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="166">
-        <v>6.8869999999999996</v>
+        <v>6.4550000000000001</v>
       </c>
       <c r="B13" s="125">
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="166">
-        <v>7.1079999999999997</v>
+        <v>6.5289999999999999</v>
       </c>
       <c r="B14" s="125">
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="166">
-        <v>7.2359999999999998</v>
+        <v>6.7119999999999997</v>
       </c>
       <c r="B15" s="125">
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="166">
-        <v>7.26</v>
+        <v>6.8869999999999996</v>
       </c>
       <c r="B16" s="125">
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="166">
-        <v>7.3710000000000004</v>
+        <v>7.1079999999999997</v>
       </c>
       <c r="B17" s="125">
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="166">
-        <v>7.4859999999999998</v>
+        <v>7.2359999999999998</v>
       </c>
       <c r="B18" s="125">
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="166">
-        <v>7.7039999999999997</v>
+        <v>7.26</v>
       </c>
       <c r="B19" s="125">
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="166">
-        <v>7.7169999999999996</v>
+        <v>7.3710000000000004</v>
       </c>
       <c r="B20" s="125">
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="166">
-        <v>7.75</v>
+        <v>7.4859999999999998</v>
       </c>
       <c r="B21" s="125">
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="166">
-        <v>8.8819999999999997</v>
+        <v>7.7169999999999996</v>
       </c>
       <c r="B22" s="125">
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="166">
-        <v>8.8970000000000002</v>
+        <v>7.75</v>
       </c>
       <c r="B23" s="125">
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="166">
-        <v>11.073</v>
+        <v>8.8819999999999997</v>
       </c>
       <c r="B24" s="125">
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8868,7 +8868,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8880,7 +8880,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8892,7 +8892,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8902,7 +8902,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8912,7 +8912,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8922,7 +8922,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8932,7 +8932,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8942,7 +8942,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8952,7 +8952,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8962,7 +8962,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C65" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -8972,7 +8972,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8982,7 +8982,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8992,7 +8992,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9002,7 +9002,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9012,7 +9012,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9022,7 +9022,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9032,7 +9032,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9042,7 +9042,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9052,7 +9052,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9062,7 +9062,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9072,7 +9072,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9082,7 +9082,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9092,7 +9092,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9102,7 +9102,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9112,7 +9112,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9122,7 +9122,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9132,14 +9132,14 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition ref="A1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9191,49 +9191,49 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>11.923999999999999</v>
+        <v>17.132999999999999</v>
       </c>
       <c r="B2" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <v>17.132999999999999</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>34.356999999999999</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="51">
         <f>'Charge 17'!F5</f>
-        <v>68.067999999999998</v>
+        <v>34.363</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="125">
-        <v>12.84</v>
+        <v>17.224</v>
       </c>
       <c r="B3" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17.224</v>
       </c>
       <c r="E3" s="50" t="s">
         <v>105</v>
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>34.356999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="125">
-        <v>16.696999999999999</v>
+        <v>11.923999999999999</v>
       </c>
       <c r="B4" s="125">
         <v>0</v>
@@ -9247,12 +9247,12 @@
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>-68.067999999999998</v>
+        <v>-6.0000000000002274E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="125">
-        <v>17.132999999999999</v>
+        <v>12.84</v>
       </c>
       <c r="B5" s="125">
         <v>0</v>
@@ -9264,7 +9264,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="125">
-        <v>17.224</v>
+        <v>16.696999999999999</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
@@ -9751,7 +9751,7 @@
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition ref="A1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9768,7 +9768,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9803,25 +9803,25 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>0</v>
+        <v>3.5110000000000001</v>
       </c>
       <c r="B2" s="125">
         <v>1</v>
       </c>
       <c r="C2">
         <f>IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <v>3.5110000000000001</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>3.5110000000000001</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="51">
         <f>'Charge 17'!F6</f>
-        <v>6.9539999999999997</v>
+        <v>3.5110000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9838,7 +9838,7 @@
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>3.5110000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9855,7 +9855,7 @@
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>-6.9539999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>